<commit_message>
add new plots to ui
</commit_message>
<xml_diff>
--- a/Misc/BioEcon_Parameters.xlsx
+++ b/Misc/BioEcon_Parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="150">
   <si>
     <t>iterations</t>
   </si>
@@ -83,9 +83,6 @@
     <t>default value</t>
   </si>
   <si>
-    <t>code name</t>
-  </si>
-  <si>
     <t>simulationYears</t>
   </si>
   <si>
@@ -411,9 +408,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>19% of rabid bites without PEP result in death, (1-0.91)*0.19=0.017</t>
   </si>
   <si>
     <t>mean abundance over observation period</t>
@@ -491,6 +485,9 @@
   </si>
   <si>
     <t>Hampson et al. 2015, SACAC 2012</t>
+  </si>
+  <si>
+    <t>variable name</t>
   </si>
 </sst>
 </file>
@@ -1211,19 +1208,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="59.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="56.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" style="2"/>
     <col min="9" max="10" width="8.83203125" style="1"/>
     <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
@@ -1232,10 +1229,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>18</v>
+        <v>149</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>13</v>
@@ -1247,15 +1244,15 @@
         <v>17</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -1266,10 +1263,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>3</v>
@@ -1281,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G3" s="13"/>
     </row>
@@ -1290,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
@@ -1302,13 +1299,13 @@
         <v>5</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -1319,10 +1316,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>4</v>
@@ -1334,18 +1331,18 @@
         <v>404</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>4</v>
@@ -1357,18 +1354,18 @@
         <v>0.49</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>4</v>
@@ -1380,18 +1377,18 @@
         <v>0.39</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>3</v>
@@ -1403,18 +1400,18 @@
         <v>0.38</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>3</v>
@@ -1426,18 +1423,18 @@
         <v>0</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>3</v>
@@ -1449,18 +1446,18 @@
         <v>0</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>3</v>
@@ -1472,18 +1469,18 @@
         <v>0</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>3</v>
@@ -1495,15 +1492,15 @@
         <v>0</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="33"/>
@@ -1514,10 +1511,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>3</v>
@@ -1529,18 +1526,18 @@
         <v>299</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>3</v>
@@ -1552,18 +1549,18 @@
         <v>89</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>3</v>
@@ -1575,15 +1572,15 @@
         <v>4000</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>1</v>
@@ -1598,18 +1595,18 @@
         <v>577</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>4</v>
@@ -1621,18 +1618,18 @@
         <v>0.9</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>4</v>
@@ -1644,18 +1641,18 @@
         <v>0.63</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>4</v>
@@ -1667,18 +1664,18 @@
         <v>0.32</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>4</v>
@@ -1690,18 +1687,18 @@
         <v>0</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>4</v>
@@ -1713,18 +1710,18 @@
         <v>189</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>4</v>
@@ -1736,15 +1733,15 @@
         <v>0.31</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>2</v>
@@ -1759,18 +1756,18 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>3</v>
@@ -1782,18 +1779,18 @@
         <v>0.38</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>4</v>
@@ -1805,38 +1802,38 @@
         <v>0</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
@@ -1851,7 +1848,7 @@
         <v>5</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>4</v>
@@ -1863,18 +1860,18 @@
         <v>0</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>4</v>
@@ -1886,15 +1883,15 @@
         <v>0</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>6</v>
@@ -1909,15 +1906,15 @@
         <v>0</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>7</v>
@@ -1932,15 +1929,15 @@
         <v>22</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>8</v>
@@ -1955,15 +1952,15 @@
         <v>3</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>9</v>
@@ -1978,15 +1975,15 @@
         <v>0</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>10</v>
@@ -2001,15 +1998,15 @@
         <v>2.15</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>11</v>
@@ -2024,15 +2021,15 @@
         <v>1.33</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>12</v>
@@ -2047,15 +2044,15 @@
         <v>0.49</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
@@ -2067,10 +2064,10 @@
     </row>
     <row r="40" spans="1:8" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>4</v>
@@ -2082,18 +2079,18 @@
         <v>1.7000000000000001E-4</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>4</v>
@@ -2105,18 +2102,18 @@
         <v>6.7559999999999995E-2</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>4</v>
@@ -2128,18 +2125,18 @@
         <v>0.99099999999999999</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>4</v>
@@ -2151,18 +2148,18 @@
         <v>0.99099999999999999</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>4</v>
@@ -2174,18 +2171,18 @@
         <v>754.92</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>4</v>
@@ -2194,18 +2191,18 @@
         <v>16</v>
       </c>
       <c r="E45" s="8">
-        <v>1.7100000000000001E-2</v>
+        <v>0.19</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
@@ -2217,10 +2214,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>4</v>
@@ -2232,18 +2229,18 @@
         <v>2.4260000000000002</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>4</v>
@@ -2255,18 +2252,18 @@
         <v>150</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>4</v>
@@ -2278,18 +2275,18 @@
         <v>150</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>4</v>
@@ -2301,18 +2298,18 @@
         <v>300</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>4</v>
@@ -2324,18 +2321,18 @@
         <v>200</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>4</v>
@@ -2347,18 +2344,18 @@
         <v>30</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>4</v>
@@ -2370,18 +2367,18 @@
         <v>2.5</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>4</v>
@@ -2393,18 +2390,18 @@
         <v>4</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>4</v>
@@ -2416,18 +2413,18 @@
         <v>2</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>4</v>
@@ -2439,18 +2436,18 @@
         <v>2</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>4</v>
@@ -2463,18 +2460,18 @@
         <v>1019.09</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G57" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>4</v>
@@ -2487,18 +2484,18 @@
         <v>2757.3</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>4</v>
@@ -2511,18 +2508,18 @@
         <v>4735.8900000000003</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G59" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C60" s="25" t="s">
         <v>4</v>
@@ -2535,10 +2532,10 @@
         <v>8453.7000000000007</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G60" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>